<commit_message>
publications added into the model.
</commit_message>
<xml_diff>
--- a/tabular/contributed/180309 GLE PIB TABLE.xlsx
+++ b/tabular/contributed/180309 GLE PIB TABLE.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12980" yWindow="1720" windowWidth="41640" windowHeight="24960" activeTab="1"/>
+    <workbookView xWindow="8340" yWindow="1720" windowWidth="41640" windowHeight="24960"/>
   </bookViews>
   <sheets>
     <sheet name="GLE" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2323" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2323" uniqueCount="139">
   <si>
     <t>Substitution</t>
   </si>
@@ -442,6 +442,12 @@
   </si>
   <si>
     <t>trialNotes</t>
+  </si>
+  <si>
+    <t>EASL_2017_FRI_205</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EASL_2017_FRI_205 </t>
   </si>
 </sst>
 </file>
@@ -1031,7 +1037,7 @@
   </sheetPr>
   <dimension ref="A1:M59"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
     </sheetView>
@@ -2344,7 +2350,7 @@
         <v>38</v>
       </c>
       <c r="K35" s="25" t="s">
-        <v>72</v>
+        <v>138</v>
       </c>
       <c r="L35" s="20"/>
       <c r="M35" s="19"/>
@@ -2381,7 +2387,7 @@
         <v>38</v>
       </c>
       <c r="K36" s="25" t="s">
-        <v>72</v>
+        <v>138</v>
       </c>
       <c r="L36" s="20"/>
       <c r="M36" s="19"/>
@@ -2418,7 +2424,7 @@
         <v>38</v>
       </c>
       <c r="K37" s="25" t="s">
-        <v>72</v>
+        <v>138</v>
       </c>
       <c r="L37" s="20"/>
       <c r="M37" s="19"/>
@@ -2455,7 +2461,7 @@
         <v>38</v>
       </c>
       <c r="K38" s="25" t="s">
-        <v>72</v>
+        <v>138</v>
       </c>
       <c r="L38" s="20"/>
       <c r="M38" s="19"/>
@@ -2492,7 +2498,7 @@
         <v>38</v>
       </c>
       <c r="K39" s="25" t="s">
-        <v>72</v>
+        <v>138</v>
       </c>
       <c r="L39" s="20"/>
       <c r="M39" s="19"/>
@@ -2529,7 +2535,7 @@
         <v>38</v>
       </c>
       <c r="K40" s="25" t="s">
-        <v>72</v>
+        <v>138</v>
       </c>
       <c r="L40" s="20"/>
       <c r="M40" s="19"/>
@@ -2566,7 +2572,7 @@
         <v>38</v>
       </c>
       <c r="K41" s="25" t="s">
-        <v>72</v>
+        <v>138</v>
       </c>
       <c r="L41" s="20"/>
       <c r="M41" s="19"/>
@@ -2603,7 +2609,7 @@
         <v>38</v>
       </c>
       <c r="K42" s="25" t="s">
-        <v>72</v>
+        <v>138</v>
       </c>
       <c r="L42" s="20"/>
       <c r="M42" s="19"/>
@@ -2640,7 +2646,7 @@
         <v>38</v>
       </c>
       <c r="K43" s="25" t="s">
-        <v>72</v>
+        <v>138</v>
       </c>
       <c r="L43" s="20"/>
       <c r="M43" s="19"/>
@@ -2677,7 +2683,7 @@
         <v>38</v>
       </c>
       <c r="K44" s="25" t="s">
-        <v>72</v>
+        <v>138</v>
       </c>
       <c r="L44" s="20"/>
       <c r="M44" s="19"/>
@@ -2714,7 +2720,7 @@
         <v>38</v>
       </c>
       <c r="K45" s="25" t="s">
-        <v>72</v>
+        <v>138</v>
       </c>
       <c r="L45" s="20"/>
       <c r="M45" s="19"/>
@@ -2751,7 +2757,7 @@
         <v>38</v>
       </c>
       <c r="K46" s="13" t="s">
-        <v>72</v>
+        <v>138</v>
       </c>
       <c r="L46" s="17"/>
       <c r="M46" s="19"/>
@@ -3242,9 +3248,9 @@
   </sheetPr>
   <dimension ref="A1:L59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4053,7 +4059,7 @@
         <v>38</v>
       </c>
       <c r="K22" s="22" t="s">
-        <v>72</v>
+        <v>137</v>
       </c>
       <c r="L22" s="17"/>
     </row>
@@ -4089,7 +4095,7 @@
         <v>38</v>
       </c>
       <c r="K23" s="22" t="s">
-        <v>72</v>
+        <v>137</v>
       </c>
       <c r="L23" s="17"/>
     </row>
@@ -4125,7 +4131,7 @@
         <v>38</v>
       </c>
       <c r="K24" s="22" t="s">
-        <v>72</v>
+        <v>137</v>
       </c>
       <c r="L24" s="17"/>
     </row>
@@ -4161,7 +4167,7 @@
         <v>38</v>
       </c>
       <c r="K25" s="22" t="s">
-        <v>72</v>
+        <v>137</v>
       </c>
       <c r="L25" s="17"/>
     </row>
@@ -4197,7 +4203,7 @@
         <v>38</v>
       </c>
       <c r="K26" s="22" t="s">
-        <v>72</v>
+        <v>137</v>
       </c>
       <c r="L26" s="17"/>
     </row>
@@ -4233,7 +4239,7 @@
         <v>38</v>
       </c>
       <c r="K27" s="22" t="s">
-        <v>72</v>
+        <v>137</v>
       </c>
       <c r="L27" s="17"/>
     </row>
@@ -4269,7 +4275,7 @@
         <v>38</v>
       </c>
       <c r="K28" s="22" t="s">
-        <v>72</v>
+        <v>137</v>
       </c>
       <c r="L28" s="17"/>
     </row>
@@ -4305,7 +4311,7 @@
         <v>38</v>
       </c>
       <c r="K29" s="22" t="s">
-        <v>72</v>
+        <v>137</v>
       </c>
       <c r="L29" s="17"/>
     </row>
@@ -4341,7 +4347,7 @@
         <v>38</v>
       </c>
       <c r="K30" s="22" t="s">
-        <v>72</v>
+        <v>137</v>
       </c>
       <c r="L30" s="17"/>
     </row>
@@ -4377,7 +4383,7 @@
         <v>38</v>
       </c>
       <c r="K31" s="22" t="s">
-        <v>72</v>
+        <v>137</v>
       </c>
       <c r="L31" s="17"/>
     </row>
@@ -4413,7 +4419,7 @@
         <v>38</v>
       </c>
       <c r="K32" s="22" t="s">
-        <v>72</v>
+        <v>137</v>
       </c>
       <c r="L32" s="17"/>
     </row>
@@ -4449,7 +4455,7 @@
         <v>38</v>
       </c>
       <c r="K33" s="22" t="s">
-        <v>72</v>
+        <v>137</v>
       </c>
       <c r="L33" s="17"/>
     </row>
@@ -4485,7 +4491,7 @@
         <v>38</v>
       </c>
       <c r="K34" s="22" t="s">
-        <v>72</v>
+        <v>137</v>
       </c>
       <c r="L34" s="17"/>
     </row>
@@ -4521,7 +4527,7 @@
         <v>38</v>
       </c>
       <c r="K35" s="22" t="s">
-        <v>72</v>
+        <v>137</v>
       </c>
       <c r="L35" s="17"/>
     </row>

</xml_diff>

<commit_message>
some cleanup tasks relating to clinical trials.
</commit_message>
<xml_diff>
--- a/tabular/contributed/180309 GLE PIB TABLE.xlsx
+++ b/tabular/contributed/180309 GLE PIB TABLE.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8340" yWindow="1720" windowWidth="41640" windowHeight="24960"/>
+    <workbookView xWindow="8300" yWindow="1720" windowWidth="41640" windowHeight="24960"/>
   </bookViews>
   <sheets>
     <sheet name="GLE" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2323" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2323" uniqueCount="141">
   <si>
     <t>Substitution</t>
   </si>
@@ -375,9 +375,6 @@
     <t>168K</t>
   </si>
   <si>
-    <t>Surveyor-1 and -2</t>
-  </si>
-  <si>
     <t>28G+30R</t>
   </si>
   <si>
@@ -448,6 +445,15 @@
   </si>
   <si>
     <t xml:space="preserve">EASL_2017_FRI_205 </t>
+  </si>
+  <si>
+    <t>Magellan-1_Part_1</t>
+  </si>
+  <si>
+    <t>Magellan-1_Part_2</t>
+  </si>
+  <si>
+    <t>Surveyor-1_and_2</t>
   </si>
 </sst>
 </file>
@@ -1038,8 +1044,8 @@
   <dimension ref="A1:M59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G59" sqref="G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1060,25 +1066,25 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="F1" s="7" t="s">
-        <v>132</v>
-      </c>
       <c r="G1" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>15</v>
@@ -1090,7 +1096,7 @@
         <v>16</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L1" s="8" t="s">
         <v>17</v>
@@ -2350,7 +2356,7 @@
         <v>38</v>
       </c>
       <c r="K35" s="25" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L35" s="20"/>
       <c r="M35" s="19"/>
@@ -2387,7 +2393,7 @@
         <v>38</v>
       </c>
       <c r="K36" s="25" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L36" s="20"/>
       <c r="M36" s="19"/>
@@ -2424,7 +2430,7 @@
         <v>38</v>
       </c>
       <c r="K37" s="25" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L37" s="20"/>
       <c r="M37" s="19"/>
@@ -2461,7 +2467,7 @@
         <v>38</v>
       </c>
       <c r="K38" s="25" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L38" s="20"/>
       <c r="M38" s="19"/>
@@ -2498,7 +2504,7 @@
         <v>38</v>
       </c>
       <c r="K39" s="25" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L39" s="20"/>
       <c r="M39" s="19"/>
@@ -2535,7 +2541,7 @@
         <v>38</v>
       </c>
       <c r="K40" s="25" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L40" s="20"/>
       <c r="M40" s="19"/>
@@ -2572,7 +2578,7 @@
         <v>38</v>
       </c>
       <c r="K41" s="25" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L41" s="20"/>
       <c r="M41" s="19"/>
@@ -2609,7 +2615,7 @@
         <v>38</v>
       </c>
       <c r="K42" s="25" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L42" s="20"/>
       <c r="M42" s="19"/>
@@ -2646,7 +2652,7 @@
         <v>38</v>
       </c>
       <c r="K43" s="25" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L43" s="20"/>
       <c r="M43" s="19"/>
@@ -2683,7 +2689,7 @@
         <v>38</v>
       </c>
       <c r="K44" s="25" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L44" s="20"/>
       <c r="M44" s="19"/>
@@ -2720,7 +2726,7 @@
         <v>38</v>
       </c>
       <c r="K45" s="25" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L45" s="20"/>
       <c r="M45" s="19"/>
@@ -2757,7 +2763,7 @@
         <v>38</v>
       </c>
       <c r="K46" s="13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L46" s="17"/>
       <c r="M46" s="19"/>
@@ -2782,7 +2788,7 @@
         <v>38</v>
       </c>
       <c r="G47" s="17" t="s">
-        <v>110</v>
+        <v>138</v>
       </c>
       <c r="H47" s="28" t="s">
         <v>71</v>
@@ -2819,7 +2825,7 @@
         <v>38</v>
       </c>
       <c r="G48" s="17" t="s">
-        <v>110</v>
+        <v>138</v>
       </c>
       <c r="H48" s="28" t="s">
         <v>71</v>
@@ -2856,7 +2862,7 @@
         <v>38</v>
       </c>
       <c r="G49" s="17" t="s">
-        <v>110</v>
+        <v>138</v>
       </c>
       <c r="H49" s="28" t="s">
         <v>71</v>
@@ -2893,7 +2899,7 @@
         <v>38</v>
       </c>
       <c r="G50" s="17" t="s">
-        <v>111</v>
+        <v>139</v>
       </c>
       <c r="H50" s="28" t="s">
         <v>71</v>
@@ -2930,7 +2936,7 @@
         <v>38</v>
       </c>
       <c r="G51" s="17" t="s">
-        <v>111</v>
+        <v>139</v>
       </c>
       <c r="H51" s="28" t="s">
         <v>71</v>
@@ -2967,7 +2973,7 @@
         <v>38</v>
       </c>
       <c r="G52" s="17" t="s">
-        <v>111</v>
+        <v>139</v>
       </c>
       <c r="H52" s="28" t="s">
         <v>71</v>
@@ -3004,7 +3010,7 @@
         <v>38</v>
       </c>
       <c r="G53" s="17" t="s">
-        <v>111</v>
+        <v>139</v>
       </c>
       <c r="H53" s="28" t="s">
         <v>71</v>
@@ -3041,7 +3047,7 @@
         <v>38</v>
       </c>
       <c r="G54" s="17" t="s">
-        <v>111</v>
+        <v>139</v>
       </c>
       <c r="H54" s="28" t="s">
         <v>71</v>
@@ -3078,7 +3084,7 @@
         <v>38</v>
       </c>
       <c r="G55" s="17" t="s">
-        <v>111</v>
+        <v>139</v>
       </c>
       <c r="H55" s="28" t="s">
         <v>71</v>
@@ -3115,7 +3121,7 @@
         <v>38</v>
       </c>
       <c r="G56" s="17" t="s">
-        <v>111</v>
+        <v>139</v>
       </c>
       <c r="H56" s="28" t="s">
         <v>71</v>
@@ -3152,7 +3158,7 @@
         <v>38</v>
       </c>
       <c r="G57" s="17" t="s">
-        <v>111</v>
+        <v>139</v>
       </c>
       <c r="H57" s="28" t="s">
         <v>71</v>
@@ -3189,7 +3195,7 @@
         <v>38</v>
       </c>
       <c r="G58" s="17" t="s">
-        <v>111</v>
+        <v>139</v>
       </c>
       <c r="H58" s="28" t="s">
         <v>71</v>
@@ -3226,7 +3232,7 @@
         <v>38</v>
       </c>
       <c r="G59" s="46" t="s">
-        <v>114</v>
+        <v>140</v>
       </c>
       <c r="H59" s="46"/>
       <c r="I59" s="46"/>
@@ -3249,8 +3255,8 @@
   <dimension ref="A1:L59"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="A1:XFD1048576"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H41" sqref="H41:H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3271,37 +3277,37 @@
   <sheetData>
     <row r="1" spans="1:12" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="K1" s="6" t="s">
         <v>132</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>133</v>
       </c>
       <c r="L1" s="8" t="s">
         <v>17</v>
@@ -4059,7 +4065,7 @@
         <v>38</v>
       </c>
       <c r="K22" s="22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L22" s="17"/>
     </row>
@@ -4095,7 +4101,7 @@
         <v>38</v>
       </c>
       <c r="K23" s="22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L23" s="17"/>
     </row>
@@ -4131,7 +4137,7 @@
         <v>38</v>
       </c>
       <c r="K24" s="22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L24" s="17"/>
     </row>
@@ -4167,7 +4173,7 @@
         <v>38</v>
       </c>
       <c r="K25" s="22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L25" s="17"/>
     </row>
@@ -4203,7 +4209,7 @@
         <v>38</v>
       </c>
       <c r="K26" s="22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L26" s="17"/>
     </row>
@@ -4239,7 +4245,7 @@
         <v>38</v>
       </c>
       <c r="K27" s="22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L27" s="17"/>
     </row>
@@ -4275,7 +4281,7 @@
         <v>38</v>
       </c>
       <c r="K28" s="22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L28" s="17"/>
     </row>
@@ -4311,7 +4317,7 @@
         <v>38</v>
       </c>
       <c r="K29" s="22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L29" s="17"/>
     </row>
@@ -4347,7 +4353,7 @@
         <v>38</v>
       </c>
       <c r="K30" s="22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L30" s="17"/>
     </row>
@@ -4383,7 +4389,7 @@
         <v>38</v>
       </c>
       <c r="K31" s="22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L31" s="17"/>
     </row>
@@ -4419,7 +4425,7 @@
         <v>38</v>
       </c>
       <c r="K32" s="22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L32" s="17"/>
     </row>
@@ -4455,7 +4461,7 @@
         <v>38</v>
       </c>
       <c r="K33" s="22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L33" s="17"/>
     </row>
@@ -4491,7 +4497,7 @@
         <v>38</v>
       </c>
       <c r="K34" s="22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L34" s="17"/>
     </row>
@@ -4527,7 +4533,7 @@
         <v>38</v>
       </c>
       <c r="K35" s="22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L35" s="17"/>
     </row>
@@ -4551,7 +4557,7 @@
         <v>38</v>
       </c>
       <c r="G36" s="17" t="s">
-        <v>110</v>
+        <v>138</v>
       </c>
       <c r="H36" s="13" t="s">
         <v>71</v>
@@ -4587,7 +4593,7 @@
         <v>38</v>
       </c>
       <c r="G37" s="17" t="s">
-        <v>110</v>
+        <v>138</v>
       </c>
       <c r="H37" s="13" t="s">
         <v>71</v>
@@ -4623,7 +4629,7 @@
         <v>38</v>
       </c>
       <c r="G38" s="17" t="s">
-        <v>110</v>
+        <v>138</v>
       </c>
       <c r="H38" s="13" t="s">
         <v>71</v>
@@ -4659,7 +4665,7 @@
         <v>38</v>
       </c>
       <c r="G39" s="17" t="s">
-        <v>110</v>
+        <v>138</v>
       </c>
       <c r="H39" s="13" t="s">
         <v>71</v>
@@ -4695,7 +4701,7 @@
         <v>38</v>
       </c>
       <c r="G40" s="17" t="s">
-        <v>111</v>
+        <v>139</v>
       </c>
       <c r="H40" s="13" t="s">
         <v>71</v>
@@ -4731,7 +4737,7 @@
         <v>38</v>
       </c>
       <c r="G41" s="17" t="s">
-        <v>111</v>
+        <v>139</v>
       </c>
       <c r="H41" s="13" t="s">
         <v>71</v>
@@ -4767,7 +4773,7 @@
         <v>38</v>
       </c>
       <c r="G42" s="17" t="s">
-        <v>111</v>
+        <v>139</v>
       </c>
       <c r="H42" s="13" t="s">
         <v>71</v>
@@ -4803,7 +4809,7 @@
         <v>38</v>
       </c>
       <c r="G43" s="17" t="s">
-        <v>111</v>
+        <v>139</v>
       </c>
       <c r="H43" s="13" t="s">
         <v>71</v>
@@ -4824,7 +4830,7 @@
         <v>36</v>
       </c>
       <c r="B44" s="40" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C44" s="40" t="s">
         <v>12</v>
@@ -4839,7 +4845,7 @@
         <v>38</v>
       </c>
       <c r="G44" s="42" t="s">
-        <v>111</v>
+        <v>139</v>
       </c>
       <c r="H44" s="40" t="s">
         <v>71</v>
@@ -4875,7 +4881,7 @@
         <v>38</v>
       </c>
       <c r="G45" s="17" t="s">
-        <v>111</v>
+        <v>139</v>
       </c>
       <c r="H45" s="13" t="s">
         <v>71</v>
@@ -4911,7 +4917,7 @@
         <v>38</v>
       </c>
       <c r="G46" s="17" t="s">
-        <v>111</v>
+        <v>139</v>
       </c>
       <c r="H46" s="13" t="s">
         <v>71</v>
@@ -4947,7 +4953,7 @@
         <v>38</v>
       </c>
       <c r="G47" s="17" t="s">
-        <v>111</v>
+        <v>139</v>
       </c>
       <c r="H47" s="13" t="s">
         <v>71</v>
@@ -4983,7 +4989,7 @@
         <v>38</v>
       </c>
       <c r="G48" s="42" t="s">
-        <v>111</v>
+        <v>139</v>
       </c>
       <c r="H48" s="40" t="s">
         <v>71</v>
@@ -5019,7 +5025,7 @@
         <v>38</v>
       </c>
       <c r="G49" s="17" t="s">
-        <v>111</v>
+        <v>139</v>
       </c>
       <c r="H49" s="13" t="s">
         <v>71</v>
@@ -5055,7 +5061,7 @@
         <v>38</v>
       </c>
       <c r="G50" s="17" t="s">
-        <v>111</v>
+        <v>139</v>
       </c>
       <c r="H50" s="13" t="s">
         <v>71</v>
@@ -5091,7 +5097,7 @@
         <v>38</v>
       </c>
       <c r="G51" s="17" t="s">
-        <v>111</v>
+        <v>139</v>
       </c>
       <c r="H51" s="13" t="s">
         <v>71</v>
@@ -5112,7 +5118,7 @@
         <v>36</v>
       </c>
       <c r="B52" s="40" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C52" s="40" t="s">
         <v>12</v>
@@ -5127,7 +5133,7 @@
         <v>38</v>
       </c>
       <c r="G52" s="42" t="s">
-        <v>111</v>
+        <v>139</v>
       </c>
       <c r="H52" s="40" t="s">
         <v>71</v>
@@ -5163,7 +5169,7 @@
         <v>38</v>
       </c>
       <c r="G53" s="17" t="s">
-        <v>111</v>
+        <v>139</v>
       </c>
       <c r="H53" s="13" t="s">
         <v>71</v>
@@ -5199,7 +5205,7 @@
         <v>38</v>
       </c>
       <c r="G54" s="17" t="s">
-        <v>111</v>
+        <v>139</v>
       </c>
       <c r="H54" s="13" t="s">
         <v>71</v>
@@ -5235,7 +5241,7 @@
         <v>38</v>
       </c>
       <c r="G55" s="17" t="s">
-        <v>111</v>
+        <v>139</v>
       </c>
       <c r="H55" s="13" t="s">
         <v>71</v>
@@ -5271,7 +5277,7 @@
         <v>38</v>
       </c>
       <c r="G56" s="17" t="s">
-        <v>111</v>
+        <v>139</v>
       </c>
       <c r="H56" s="13" t="s">
         <v>71</v>
@@ -5406,7 +5412,7 @@
   <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A2" sqref="A2:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5416,47 +5422,47 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="49" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>